<commit_message>
Mod Part Patching for 0.8.0
</commit_message>
<xml_diff>
--- a/Plotting/0.7.5/HabTech2.xlsx
+++ b/Plotting/0.7.5/HabTech2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.7.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.7.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026BC504-7CEE-4D1D-A10D-44F627C83D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7410D8EE-1A2A-4E22-AD23-BC6F29931FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="15132" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3276" yWindow="960" windowWidth="15228" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HabTech2" sheetId="1" r:id="rId1"/>
@@ -33,87 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
-    <t>PART.name</t>
-  </si>
-  <si>
-    <t>ht2.CBM</t>
-  </si>
-  <si>
-    <t>ht2.handrail</t>
-  </si>
-  <si>
-    <t>ht2.JEM.EF</t>
-  </si>
-  <si>
-    <t>ht2.moduleColumbus</t>
-  </si>
-  <si>
-    <t>ht2.moduleCupola</t>
-  </si>
-  <si>
-    <t>ht2.moduleDestiny</t>
-  </si>
-  <si>
-    <t>ht2.moduleHarmony</t>
-  </si>
-  <si>
-    <t>ht2.moduleJEMlogistics</t>
-  </si>
-  <si>
-    <t>ht2.moduleKibo</t>
-  </si>
-  <si>
-    <t>ht2.moduleLabNode</t>
-  </si>
-  <si>
-    <t>ht2.moduleQuest</t>
-  </si>
-  <si>
-    <t>ht2.moduleUnity</t>
-  </si>
-  <si>
-    <t>ht2.MPLM</t>
-  </si>
-  <si>
-    <t>ht2.MPLM.half</t>
-  </si>
-  <si>
-    <t>ht2.PMA</t>
-  </si>
-  <si>
-    <t>ht2.questPod</t>
-  </si>
-  <si>
-    <t>ht2.questRack</t>
-  </si>
-  <si>
-    <t>ht2.radialTrussPort</t>
-  </si>
-  <si>
-    <t>ht2.radiatorTriple</t>
-  </si>
-  <si>
-    <t>ht2.solarArray.duo</t>
-  </si>
-  <si>
-    <t>ht2.solarArray.solo</t>
-  </si>
-  <si>
-    <t>ht2.trussPort</t>
-  </si>
-  <si>
-    <t>ht2.truss.S0</t>
-  </si>
-  <si>
-    <t>ht2.truss.S1</t>
-  </si>
-  <si>
-    <t>ht2.truss.S2</t>
-  </si>
-  <si>
-    <t>ht2.truss.Z1</t>
-  </si>
-  <si>
     <t>SSS Category</t>
   </si>
   <si>
@@ -214,6 +133,87 @@
   </si>
   <si>
     <t>construction</t>
+  </si>
+  <si>
+    <t>PART_name</t>
+  </si>
+  <si>
+    <t>ht2_radialTrussPort</t>
+  </si>
+  <si>
+    <t>ht2_trussPort</t>
+  </si>
+  <si>
+    <t>ht2_truss_S0</t>
+  </si>
+  <si>
+    <t>ht2_truss_S1</t>
+  </si>
+  <si>
+    <t>ht2_truss_S2</t>
+  </si>
+  <si>
+    <t>ht2_truss_Z1</t>
+  </si>
+  <si>
+    <t>ht2_moduleJEMlogistics</t>
+  </si>
+  <si>
+    <t>ht2_MPLM</t>
+  </si>
+  <si>
+    <t>ht2_MPLM_half</t>
+  </si>
+  <si>
+    <t>ht2_questPod</t>
+  </si>
+  <si>
+    <t>ht2_questRack</t>
+  </si>
+  <si>
+    <t>ht2_solarArray_duo</t>
+  </si>
+  <si>
+    <t>ht2_solarArray_solo</t>
+  </si>
+  <si>
+    <t>ht2_CBM</t>
+  </si>
+  <si>
+    <t>ht2_handrail</t>
+  </si>
+  <si>
+    <t>ht2_JEM_EF</t>
+  </si>
+  <si>
+    <t>ht2_moduleColumbus</t>
+  </si>
+  <si>
+    <t>ht2_moduleCupola</t>
+  </si>
+  <si>
+    <t>ht2_moduleDestiny</t>
+  </si>
+  <si>
+    <t>ht2_moduleHarmony</t>
+  </si>
+  <si>
+    <t>ht2_moduleKibo</t>
+  </si>
+  <si>
+    <t>ht2_moduleLabNode</t>
+  </si>
+  <si>
+    <t>ht2_moduleQuest</t>
+  </si>
+  <si>
+    <t>ht2_moduleUnity</t>
+  </si>
+  <si>
+    <t>ht2_PMA</t>
+  </si>
+  <si>
+    <t>ht2_radiatorTriple</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,37 +1074,37 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E2" t="str">
-        <f>"@PART["&amp;A2&amp;"]:AFTER["&amp;D2&amp;"] //
+        <f t="shared" ref="E2:E27" si="0">"@PART["&amp;A2&amp;"]:AFTER["&amp;D2&amp;"] //
 {
 	@TechRequired = "&amp;B2&amp;C2&amp;"
 }"</f>
-        <v>@PART[ht2.radialTrussPort]:AFTER[HabTech19] //
+        <v>@PART[ht2_radialTrussPort]:AFTER[HabTech19] //
 {
 	@TechRequired = construction9
 }</v>
@@ -1112,23 +1112,20 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E3" t="str">
-        <f>"@PART["&amp;A3&amp;"]:AFTER["&amp;D3&amp;"] //
-{
-	@TechRequired = "&amp;B3&amp;C3&amp;"
-}"</f>
-        <v>@PART[ht2.trussPort]:AFTER[HabTech23] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_trussPort]:AFTER[HabTech23] //
 {
 	@TechRequired = construction9
 }</v>
@@ -1136,23 +1133,20 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E4" t="str">
-        <f>"@PART["&amp;A4&amp;"]:AFTER["&amp;D4&amp;"] //
-{
-	@TechRequired = "&amp;B4&amp;C4&amp;"
-}"</f>
-        <v>@PART[ht2.truss.S0]:AFTER[HabTech24] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_truss_S0]:AFTER[HabTech24] //
 {
 	@TechRequired = construction9
 }</v>
@@ -1160,23 +1154,20 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E5" t="str">
-        <f>"@PART["&amp;A5&amp;"]:AFTER["&amp;D5&amp;"] //
-{
-	@TechRequired = "&amp;B5&amp;C5&amp;"
-}"</f>
-        <v>@PART[ht2.truss.S1]:AFTER[HabTech25] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_truss_S1]:AFTER[HabTech25] //
 {
 	@TechRequired = construction9
 }</v>
@@ -1184,23 +1175,20 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="E6" t="str">
-        <f>"@PART["&amp;A6&amp;"]:AFTER["&amp;D6&amp;"] //
-{
-	@TechRequired = "&amp;B6&amp;C6&amp;"
-}"</f>
-        <v>@PART[ht2.truss.S2]:AFTER[HabTech26] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_truss_S2]:AFTER[HabTech26] //
 {
 	@TechRequired = construction9
 }</v>
@@ -1208,23 +1196,20 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E7" t="str">
-        <f>"@PART["&amp;A7&amp;"]:AFTER["&amp;D7&amp;"] //
-{
-	@TechRequired = "&amp;B7&amp;C7&amp;"
-}"</f>
-        <v>@PART[ht2.truss.Z1]:AFTER[HabTech27] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_truss_Z1]:AFTER[HabTech27] //
 {
 	@TechRequired = construction9
 }</v>
@@ -1232,23 +1217,20 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E8" t="str">
-        <f>"@PART["&amp;A8&amp;"]:AFTER["&amp;D8&amp;"] //
-{
-	@TechRequired = "&amp;B8&amp;C8&amp;"
-}"</f>
-        <v>@PART[ht2.moduleJEMlogistics]:AFTER[HabTech9] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleJEMlogistics]:AFTER[HabTech9] //
 {
 	@TechRequired = logistics9
 }</v>
@@ -1256,23 +1238,20 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E9" t="str">
-        <f>"@PART["&amp;A9&amp;"]:AFTER["&amp;D9&amp;"] //
-{
-	@TechRequired = "&amp;B9&amp;C9&amp;"
-}"</f>
-        <v>@PART[ht2.MPLM]:AFTER[HabTech14] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_MPLM]:AFTER[HabTech14] //
 {
 	@TechRequired = logistics9
 }</v>
@@ -1280,23 +1259,20 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="E10" t="str">
-        <f>"@PART["&amp;A10&amp;"]:AFTER["&amp;D10&amp;"] //
-{
-	@TechRequired = "&amp;B10&amp;C10&amp;"
-}"</f>
-        <v>@PART[ht2.MPLM.half]:AFTER[HabTech15] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_MPLM_half]:AFTER[HabTech15] //
 {
 	@TechRequired = logistics9
 }</v>
@@ -1304,23 +1280,20 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E11" t="str">
-        <f>"@PART["&amp;A11&amp;"]:AFTER["&amp;D11&amp;"] //
-{
-	@TechRequired = "&amp;B11&amp;C11&amp;"
-}"</f>
-        <v>@PART[ht2.questPod]:AFTER[HabTech17] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_questPod]:AFTER[HabTech17] //
 {
 	@TechRequired = logistics9
 }</v>
@@ -1328,23 +1301,20 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E12" t="str">
-        <f>"@PART["&amp;A12&amp;"]:AFTER["&amp;D12&amp;"] //
-{
-	@TechRequired = "&amp;B12&amp;C12&amp;"
-}"</f>
-        <v>@PART[ht2.questRack]:AFTER[HabTech18] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_questRack]:AFTER[HabTech18] //
 {
 	@TechRequired = logistics9
 }</v>
@@ -1352,47 +1322,41 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="str">
-        <f>"@PART["&amp;A13&amp;"]:AFTER["&amp;D13&amp;"] //
+        <v>22</v>
+      </c>
+      <c r="E13" t="b">
+        <f>B7="@PART["&amp;A13&amp;"]:AFTER["&amp;D13&amp;"] //
 {
 	@TechRequired = "&amp;B13&amp;C13&amp;"
 }"</f>
-        <v>@PART[ht2.solarArray.duo]:AFTER[HabTech21] //
-{
-	@TechRequired = solar9
-}</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E14" t="str">
-        <f>"@PART["&amp;A14&amp;"]:AFTER["&amp;D14&amp;"] //
-{
-	@TechRequired = "&amp;B14&amp;C14&amp;"
-}"</f>
-        <v>@PART[ht2.solarArray.solo]:AFTER[HabTech22] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_solarArray_solo]:AFTER[HabTech22] //
 {
 	@TechRequired = solar9
 }</v>
@@ -1400,23 +1364,20 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E15" t="str">
-        <f>"@PART["&amp;A15&amp;"]:AFTER["&amp;D15&amp;"] //
-{
-	@TechRequired = "&amp;B15&amp;C15&amp;"
-}"</f>
-        <v>@PART[ht2.CBM]:AFTER[HabTech2] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_CBM]:AFTER[HabTech2] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1424,23 +1385,20 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="E16" t="str">
-        <f>"@PART["&amp;A16&amp;"]:AFTER["&amp;D16&amp;"] //
-{
-	@TechRequired = "&amp;B16&amp;C16&amp;"
-}"</f>
-        <v>@PART[ht2.handrail]:AFTER[HabTech3] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_handrail]:AFTER[HabTech3] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1448,23 +1406,20 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="E17" t="str">
-        <f>"@PART["&amp;A17&amp;"]:AFTER["&amp;D17&amp;"] //
-{
-	@TechRequired = "&amp;B17&amp;C17&amp;"
-}"</f>
-        <v>@PART[ht2.JEM.EF]:AFTER[HabTech4] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_JEM_EF]:AFTER[HabTech4] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1472,23 +1427,20 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E18" t="str">
-        <f>"@PART["&amp;A18&amp;"]:AFTER["&amp;D18&amp;"] //
-{
-	@TechRequired = "&amp;B18&amp;C18&amp;"
-}"</f>
-        <v>@PART[ht2.moduleColumbus]:AFTER[HabTech5] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleColumbus]:AFTER[HabTech5] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1496,23 +1448,20 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E19" t="str">
-        <f>"@PART["&amp;A19&amp;"]:AFTER["&amp;D19&amp;"] //
-{
-	@TechRequired = "&amp;B19&amp;C19&amp;"
-}"</f>
-        <v>@PART[ht2.moduleCupola]:AFTER[HabTech6] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleCupola]:AFTER[HabTech6] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1520,23 +1469,20 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E20" t="str">
-        <f>"@PART["&amp;A20&amp;"]:AFTER["&amp;D20&amp;"] //
-{
-	@TechRequired = "&amp;B20&amp;C20&amp;"
-}"</f>
-        <v>@PART[ht2.moduleDestiny]:AFTER[HabTech7] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleDestiny]:AFTER[HabTech7] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1544,23 +1490,20 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f>"@PART["&amp;A21&amp;"]:AFTER["&amp;D21&amp;"] //
-{
-	@TechRequired = "&amp;B21&amp;C21&amp;"
-}"</f>
-        <v>@PART[ht2.moduleHarmony]:AFTER[HabTech8] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleHarmony]:AFTER[HabTech8] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1568,23 +1511,20 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E22" t="str">
-        <f>"@PART["&amp;A22&amp;"]:AFTER["&amp;D22&amp;"] //
-{
-	@TechRequired = "&amp;B22&amp;C22&amp;"
-}"</f>
-        <v>@PART[ht2.moduleKibo]:AFTER[HabTech10] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleKibo]:AFTER[HabTech10] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1592,23 +1532,20 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E23" t="str">
-        <f>"@PART["&amp;A23&amp;"]:AFTER["&amp;D23&amp;"] //
-{
-	@TechRequired = "&amp;B23&amp;C23&amp;"
-}"</f>
-        <v>@PART[ht2.moduleLabNode]:AFTER[HabTech11] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleLabNode]:AFTER[HabTech11] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1616,23 +1553,20 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E24" t="str">
-        <f>"@PART["&amp;A24&amp;"]:AFTER["&amp;D24&amp;"] //
-{
-	@TechRequired = "&amp;B24&amp;C24&amp;"
-}"</f>
-        <v>@PART[ht2.moduleQuest]:AFTER[HabTech12] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleQuest]:AFTER[HabTech12] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1640,23 +1574,20 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E25" t="str">
-        <f>"@PART["&amp;A25&amp;"]:AFTER["&amp;D25&amp;"] //
-{
-	@TechRequired = "&amp;B25&amp;C25&amp;"
-}"</f>
-        <v>@PART[ht2.moduleUnity]:AFTER[HabTech13] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_moduleUnity]:AFTER[HabTech13] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1664,23 +1595,20 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="E26" t="str">
-        <f>"@PART["&amp;A26&amp;"]:AFTER["&amp;D26&amp;"] //
-{
-	@TechRequired = "&amp;B26&amp;C26&amp;"
-}"</f>
-        <v>@PART[ht2.PMA]:AFTER[HabTech16] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_PMA]:AFTER[HabTech16] //
 {
 	@TechRequired = spaceStations9
 }</v>
@@ -1688,23 +1616,20 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="E27" t="str">
-        <f>"@PART["&amp;A27&amp;"]:AFTER["&amp;D27&amp;"] //
-{
-	@TechRequired = "&amp;B27&amp;C27&amp;"
-}"</f>
-        <v>@PART[ht2.radiatorTriple]:AFTER[HabTech20] //
+        <f t="shared" si="0"/>
+        <v>@PART[ht2_radiatorTriple]:AFTER[HabTech20] //
 {
 	@TechRequired = thermal9
 }</v>

</xml_diff>